<commit_message>
Improve flow analyses and restructuring of the SHArC module (more will follow).
</commit_message>
<xml_diff>
--- a/.site_packages/templates/Fish.xlsx
+++ b/.site_packages/templates/Fish.xlsx
@@ -97,6 +97,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="AO80" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rad. = Radius (length either in feet or m)</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C83" authorId="0" shapeId="0">
       <text>
         <r>
@@ -145,12 +169,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="AO83" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rad. = Radius (length either in feet or m)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="60">
   <si>
     <t>Chinook Salmon</t>
   </si>
@@ -379,6 +427,30 @@
   <si>
     <t>Season end</t>
   </si>
+  <si>
+    <t>All Aquatic</t>
+  </si>
+  <si>
+    <t>Whetted area</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>DO NOT MODIFY LIFESTAGE NAMES</t>
+  </si>
+  <si>
+    <t>hydrologic year</t>
+  </si>
+  <si>
+    <t>depth &gt; x</t>
+  </si>
+  <si>
+    <t>velocity &gt; x</t>
+  </si>
 </sst>
 </file>
 
@@ -387,7 +459,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +549,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1508,8 +1588,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1540,29 +1618,16 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1591,13 +1656,28 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1623,7 +1703,7 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -1657,6 +1737,20 @@
         <name val="Arial Narrow"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1951,10 +2045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AH85"/>
+  <dimension ref="B1:AP85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1969,506 +2063,618 @@
     <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="2:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="43" t="s">
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="44" t="str">
+      <c r="L1" s="42" t="str">
         <f>IF($C1=template!$L3,"(fps)", "(m/s)")</f>
         <v>(fps)</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="44" t="str">
+      <c r="N1" s="42" t="str">
         <f>IF($C1=template!$L3,"(ft)", "(m)")</f>
         <v>(ft)</v>
       </c>
-      <c r="O1" s="43" t="s">
+      <c r="O1" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="44" t="str">
+      <c r="P1" s="42" t="str">
         <f>IF($C1=template!$L3,"(inch)", "(m)")</f>
         <v>(inch)</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="44" t="str">
+      <c r="R1" s="42" t="str">
         <f>IF($C1=template!$L3,"(ft)", "(m)")</f>
         <v>(ft)</v>
       </c>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="41"/>
-    </row>
-    <row r="2" spans="2:34" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
+      <c r="AM1" s="54"/>
+      <c r="AN1" s="54"/>
+      <c r="AO1" s="54"/>
+      <c r="AP1" s="55"/>
+    </row>
+    <row r="2" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="64" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="64" t="s">
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="64" t="s">
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
-      <c r="AE2" s="65"/>
-      <c r="AF2" s="65"/>
-      <c r="AG2" s="65"/>
-      <c r="AH2" s="66"/>
-    </row>
-    <row r="3" spans="2:34" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
+      <c r="AD2" s="60"/>
+      <c r="AE2" s="60"/>
+      <c r="AF2" s="60"/>
+      <c r="AG2" s="60"/>
+      <c r="AH2" s="61"/>
+      <c r="AI2" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ2" s="60"/>
+      <c r="AK2" s="60"/>
+      <c r="AL2" s="60"/>
+      <c r="AM2" s="60"/>
+      <c r="AN2" s="60"/>
+      <c r="AO2" s="60"/>
+      <c r="AP2" s="61"/>
+    </row>
+    <row r="3" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="67" t="s">
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
-      <c r="X3" s="68"/>
-      <c r="Y3" s="68"/>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="67" t="s">
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="62"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="AB3" s="68"/>
-      <c r="AC3" s="68"/>
-      <c r="AD3" s="68"/>
-      <c r="AE3" s="68"/>
-      <c r="AF3" s="68"/>
-      <c r="AG3" s="68"/>
-      <c r="AH3" s="69"/>
-    </row>
-    <row r="4" spans="2:34" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="52" t="s">
+      <c r="AB3" s="63"/>
+      <c r="AC3" s="63"/>
+      <c r="AD3" s="63"/>
+      <c r="AE3" s="63"/>
+      <c r="AF3" s="63"/>
+      <c r="AG3" s="63"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" s="63"/>
+      <c r="AK3" s="63"/>
+      <c r="AL3" s="63"/>
+      <c r="AM3" s="63"/>
+      <c r="AN3" s="63"/>
+      <c r="AO3" s="63"/>
+      <c r="AP3" s="64"/>
+    </row>
+    <row r="4" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="71"/>
-      <c r="U4" s="71"/>
-      <c r="V4" s="71"/>
-      <c r="W4" s="71"/>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="70" t="s">
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="AB4" s="71"/>
-      <c r="AC4" s="71"/>
-      <c r="AD4" s="71"/>
-      <c r="AE4" s="71"/>
-      <c r="AF4" s="71"/>
-      <c r="AG4" s="71"/>
-      <c r="AH4" s="72"/>
-    </row>
-    <row r="5" spans="2:34" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="55" t="s">
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="67"/>
+      <c r="AI4" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ4" s="66"/>
+      <c r="AK4" s="66"/>
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="67"/>
+    </row>
+    <row r="5" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="56" t="s">
+      <c r="D5" s="73"/>
+      <c r="E5" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="56" t="s">
+      <c r="F5" s="73"/>
+      <c r="G5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="56" t="s">
+      <c r="H5" s="73"/>
+      <c r="I5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="58" t="s">
+      <c r="J5" s="75"/>
+      <c r="K5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="56" t="s">
+      <c r="L5" s="73"/>
+      <c r="M5" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="59"/>
-      <c r="O5" s="56" t="s">
+      <c r="N5" s="73"/>
+      <c r="O5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="56" t="s">
+      <c r="P5" s="73"/>
+      <c r="Q5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="57"/>
-      <c r="S5" s="58" t="s">
+      <c r="R5" s="75"/>
+      <c r="S5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="59"/>
-      <c r="U5" s="56" t="s">
+      <c r="T5" s="73"/>
+      <c r="U5" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="59"/>
-      <c r="W5" s="56" t="s">
+      <c r="V5" s="73"/>
+      <c r="W5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="56" t="s">
+      <c r="X5" s="73"/>
+      <c r="Y5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="Z5" s="57"/>
-      <c r="AA5" s="58" t="s">
+      <c r="Z5" s="75"/>
+      <c r="AA5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="AB5" s="59"/>
-      <c r="AC5" s="56" t="s">
+      <c r="AB5" s="73"/>
+      <c r="AC5" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="AD5" s="59"/>
-      <c r="AE5" s="56" t="s">
+      <c r="AD5" s="73"/>
+      <c r="AE5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="AF5" s="59"/>
-      <c r="AG5" s="56" t="s">
+      <c r="AF5" s="73"/>
+      <c r="AG5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="AH5" s="57"/>
-    </row>
-    <row r="6" spans="2:34" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47" t="s">
+      <c r="AH5" s="75"/>
+      <c r="AI5" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ5" s="73"/>
+      <c r="AK5" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL5" s="73"/>
+      <c r="AM5" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN5" s="73"/>
+      <c r="AO5" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP5" s="75"/>
+    </row>
+    <row r="6" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="54">
+      <c r="C6" s="51"/>
+      <c r="D6" s="52">
         <v>43739</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="54">
+      <c r="E6" s="46"/>
+      <c r="F6" s="52">
         <v>43497</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="54">
+      <c r="G6" s="46"/>
+      <c r="H6" s="52">
         <v>43632</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49">
+      <c r="I6" s="46"/>
+      <c r="J6" s="47">
         <v>43739</v>
       </c>
-      <c r="K6" s="53"/>
-      <c r="L6" s="54">
+      <c r="K6" s="51"/>
+      <c r="L6" s="52">
         <v>43739</v>
       </c>
-      <c r="M6" s="48"/>
-      <c r="N6" s="54">
+      <c r="M6" s="46"/>
+      <c r="N6" s="52">
         <v>43739</v>
       </c>
-      <c r="O6" s="48"/>
-      <c r="P6" s="54">
+      <c r="O6" s="46"/>
+      <c r="P6" s="52">
         <v>43739</v>
       </c>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="49">
+      <c r="Q6" s="46"/>
+      <c r="R6" s="47">
         <v>43739</v>
       </c>
-      <c r="S6" s="53"/>
-      <c r="T6" s="54">
+      <c r="S6" s="51"/>
+      <c r="T6" s="52">
         <v>43739</v>
       </c>
-      <c r="U6" s="48"/>
-      <c r="V6" s="54">
+      <c r="U6" s="46"/>
+      <c r="V6" s="52">
         <v>43739</v>
       </c>
-      <c r="W6" s="48"/>
-      <c r="X6" s="54">
+      <c r="W6" s="46"/>
+      <c r="X6" s="52">
         <v>43739</v>
       </c>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="49">
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="47">
         <v>43739</v>
       </c>
-      <c r="AA6" s="53"/>
-      <c r="AB6" s="54">
+      <c r="AA6" s="51"/>
+      <c r="AB6" s="52">
         <v>43739</v>
       </c>
-      <c r="AC6" s="48"/>
-      <c r="AD6" s="54">
+      <c r="AC6" s="46"/>
+      <c r="AD6" s="52">
         <v>43739</v>
       </c>
-      <c r="AE6" s="48"/>
-      <c r="AF6" s="54">
+      <c r="AE6" s="46"/>
+      <c r="AF6" s="52">
         <v>43739</v>
       </c>
-      <c r="AG6" s="48"/>
-      <c r="AH6" s="49">
+      <c r="AG6" s="46"/>
+      <c r="AH6" s="47">
         <v>43739</v>
       </c>
-    </row>
-    <row r="7" spans="2:34" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47" t="s">
+      <c r="AI6" s="51"/>
+      <c r="AJ6" s="52">
+        <v>43739</v>
+      </c>
+      <c r="AK6" s="46"/>
+      <c r="AL6" s="52">
+        <v>43497</v>
+      </c>
+      <c r="AM6" s="46"/>
+      <c r="AN6" s="52">
+        <v>43739</v>
+      </c>
+      <c r="AO6" s="46"/>
+      <c r="AP6" s="47">
+        <v>43739</v>
+      </c>
+    </row>
+    <row r="7" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49">
         <v>43738</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="51">
+      <c r="E7" s="46"/>
+      <c r="F7" s="49">
         <v>43631</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="51">
+      <c r="G7" s="46"/>
+      <c r="H7" s="49">
         <v>43769</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="49">
+      <c r="I7" s="46"/>
+      <c r="J7" s="47">
         <v>43738</v>
       </c>
-      <c r="K7" s="50"/>
-      <c r="L7" s="51">
+      <c r="K7" s="48"/>
+      <c r="L7" s="49">
         <v>43738</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="51">
+      <c r="M7" s="46"/>
+      <c r="N7" s="49">
         <v>43738</v>
       </c>
-      <c r="O7" s="48"/>
-      <c r="P7" s="51">
+      <c r="O7" s="46"/>
+      <c r="P7" s="49">
         <v>43738</v>
       </c>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="49">
+      <c r="Q7" s="46"/>
+      <c r="R7" s="47">
         <v>43738</v>
       </c>
-      <c r="S7" s="50"/>
-      <c r="T7" s="51">
+      <c r="S7" s="48"/>
+      <c r="T7" s="49">
         <v>43738</v>
       </c>
-      <c r="U7" s="48"/>
-      <c r="V7" s="51">
+      <c r="U7" s="46"/>
+      <c r="V7" s="49">
         <v>43738</v>
       </c>
-      <c r="W7" s="48"/>
-      <c r="X7" s="51">
+      <c r="W7" s="46"/>
+      <c r="X7" s="49">
         <v>43738</v>
       </c>
-      <c r="Y7" s="48"/>
-      <c r="Z7" s="49">
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="47">
         <v>43738</v>
       </c>
-      <c r="AA7" s="50"/>
-      <c r="AB7" s="51">
+      <c r="AA7" s="48"/>
+      <c r="AB7" s="49">
         <v>43738</v>
       </c>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="51">
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="49">
         <v>43738</v>
       </c>
-      <c r="AE7" s="48"/>
-      <c r="AF7" s="51">
+      <c r="AE7" s="46"/>
+      <c r="AF7" s="49">
         <v>43738</v>
       </c>
-      <c r="AG7" s="48"/>
-      <c r="AH7" s="49">
+      <c r="AG7" s="46"/>
+      <c r="AH7" s="47">
         <v>43738</v>
       </c>
-    </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B8" s="60" t="s">
+      <c r="AI7" s="48"/>
+      <c r="AJ7" s="49">
+        <v>43738</v>
+      </c>
+      <c r="AK7" s="46"/>
+      <c r="AL7" s="49">
+        <v>43631</v>
+      </c>
+      <c r="AM7" s="46"/>
+      <c r="AN7" s="49">
+        <v>43738</v>
+      </c>
+      <c r="AO7" s="46"/>
+      <c r="AP7" s="47">
+        <v>43738</v>
+      </c>
+    </row>
+    <row r="8" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B8" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="43" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="I8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="J8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="43" t="s">
         <v>40</v>
       </c>
       <c r="L8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="46" t="s">
+      <c r="M8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="N8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="46" t="s">
+      <c r="O8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="P8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="46" t="s">
+      <c r="Q8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="R8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="45" t="s">
+      <c r="S8" s="43" t="s">
         <v>39</v>
       </c>
       <c r="T8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="46" t="s">
+      <c r="U8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="V8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="W8" s="46" t="s">
+      <c r="W8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="X8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Y8" s="46" t="s">
+      <c r="Y8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="Z8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AA8" s="45" t="s">
+      <c r="AA8" s="43" t="s">
         <v>39</v>
       </c>
       <c r="AB8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AC8" s="46" t="s">
+      <c r="AC8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="AD8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AE8" s="46" t="s">
+      <c r="AE8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="AF8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AG8" s="46" t="s">
+      <c r="AG8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="AH8" s="35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B9" s="61"/>
+      <c r="AI8" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK8" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM8" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO8" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP8" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B9" s="69"/>
       <c r="C9" s="30">
         <v>0.22</v>
       </c>
@@ -2541,9 +2747,33 @@
       <c r="AF9" s="31"/>
       <c r="AG9" s="32"/>
       <c r="AH9" s="33"/>
-    </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B10" s="61"/>
+      <c r="AI9" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ9" s="31">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="AL9" s="31">
+        <v>1</v>
+      </c>
+      <c r="AM9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="31">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="32">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B10" s="69"/>
       <c r="C10" s="15">
         <v>0.85</v>
       </c>
@@ -2616,9 +2846,33 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="5"/>
       <c r="AH10" s="16"/>
-    </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B11" s="61"/>
+      <c r="AI10" s="15">
+        <v>100</v>
+      </c>
+      <c r="AJ10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="5">
+        <v>100</v>
+      </c>
+      <c r="AL10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AM10" s="5">
+        <v>100</v>
+      </c>
+      <c r="AN10" s="6">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AP10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B11" s="69"/>
       <c r="C11" s="15">
         <v>1.3</v>
       </c>
@@ -2691,9 +2945,21 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="5"/>
       <c r="AH11" s="16"/>
-    </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B12" s="61"/>
+      <c r="AI11" s="15"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="6"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AP11" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B12" s="69"/>
       <c r="C12" s="15">
         <v>1.55</v>
       </c>
@@ -2766,9 +3032,21 @@
       <c r="AF12" s="6"/>
       <c r="AG12" s="5"/>
       <c r="AH12" s="16"/>
-    </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B13" s="61"/>
+      <c r="AI12" s="15"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="5"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="5">
+        <v>100</v>
+      </c>
+      <c r="AP12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B13" s="69"/>
       <c r="C13" s="15">
         <v>2.95</v>
       </c>
@@ -2833,9 +3111,17 @@
       <c r="AF13" s="6"/>
       <c r="AG13" s="5"/>
       <c r="AH13" s="16"/>
-    </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B14" s="61"/>
+      <c r="AI13" s="15"/>
+      <c r="AJ13" s="6"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="16"/>
+    </row>
+    <row r="14" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B14" s="69"/>
       <c r="C14" s="15">
         <v>3.25</v>
       </c>
@@ -2900,9 +3186,17 @@
       <c r="AF14" s="6"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="16"/>
-    </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B15" s="61"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="16"/>
+    </row>
+    <row r="15" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B15" s="69"/>
       <c r="C15" s="15">
         <v>5.32</v>
       </c>
@@ -2967,9 +3261,17 @@
       <c r="AF15" s="6"/>
       <c r="AG15" s="5"/>
       <c r="AH15" s="16"/>
-    </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B16" s="61"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="5"/>
+      <c r="AL15" s="6"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="6"/>
+      <c r="AO15" s="5"/>
+      <c r="AP15" s="16"/>
+    </row>
+    <row r="16" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B16" s="69"/>
       <c r="C16" s="15"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5">
@@ -3026,9 +3328,17 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="5"/>
       <c r="AH16" s="16"/>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B17" s="61"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="6"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="6"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="6"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="16"/>
+    </row>
+    <row r="17" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B17" s="69"/>
       <c r="C17" s="15"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5">
@@ -3081,9 +3391,17 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="5"/>
       <c r="AH17" s="16"/>
-    </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B18" s="61"/>
+      <c r="AI17" s="15"/>
+      <c r="AJ17" s="6"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="6"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="6"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="16"/>
+    </row>
+    <row r="18" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B18" s="69"/>
       <c r="C18" s="15"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5">
@@ -3136,9 +3454,17 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="5"/>
       <c r="AH18" s="16"/>
-    </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B19" s="61"/>
+      <c r="AI18" s="15"/>
+      <c r="AJ18" s="6"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="6"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="6"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="16"/>
+    </row>
+    <row r="19" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B19" s="69"/>
       <c r="C19" s="15"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5">
@@ -3187,9 +3513,17 @@
       <c r="AF19" s="6"/>
       <c r="AG19" s="5"/>
       <c r="AH19" s="16"/>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B20" s="61"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="6"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="6"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="6"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="16"/>
+    </row>
+    <row r="20" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B20" s="69"/>
       <c r="C20" s="15"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5">
@@ -3238,9 +3572,17 @@
       <c r="AF20" s="6"/>
       <c r="AG20" s="5"/>
       <c r="AH20" s="16"/>
-    </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B21" s="61"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="6"/>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="6"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="6"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="16"/>
+    </row>
+    <row r="21" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B21" s="69"/>
       <c r="C21" s="15"/>
       <c r="D21" s="6"/>
       <c r="E21" s="5">
@@ -3289,9 +3631,17 @@
       <c r="AF21" s="6"/>
       <c r="AG21" s="5"/>
       <c r="AH21" s="16"/>
-    </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B22" s="61"/>
+      <c r="AI21" s="15"/>
+      <c r="AJ21" s="6"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="16"/>
+    </row>
+    <row r="22" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B22" s="69"/>
       <c r="C22" s="15"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5">
@@ -3340,9 +3690,17 @@
       <c r="AF22" s="6"/>
       <c r="AG22" s="5"/>
       <c r="AH22" s="16"/>
-    </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B23" s="61"/>
+      <c r="AI22" s="15"/>
+      <c r="AJ22" s="6"/>
+      <c r="AK22" s="5"/>
+      <c r="AL22" s="6"/>
+      <c r="AM22" s="5"/>
+      <c r="AN22" s="6"/>
+      <c r="AO22" s="5"/>
+      <c r="AP22" s="16"/>
+    </row>
+    <row r="23" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B23" s="69"/>
       <c r="C23" s="15"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5">
@@ -3391,9 +3749,17 @@
       <c r="AF23" s="6"/>
       <c r="AG23" s="5"/>
       <c r="AH23" s="16"/>
-    </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B24" s="61"/>
+      <c r="AI23" s="15"/>
+      <c r="AJ23" s="6"/>
+      <c r="AK23" s="5"/>
+      <c r="AL23" s="6"/>
+      <c r="AM23" s="5"/>
+      <c r="AN23" s="6"/>
+      <c r="AO23" s="5"/>
+      <c r="AP23" s="16"/>
+    </row>
+    <row r="24" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B24" s="69"/>
       <c r="C24" s="15"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
@@ -3438,9 +3804,17 @@
       <c r="AF24" s="6"/>
       <c r="AG24" s="5"/>
       <c r="AH24" s="16"/>
-    </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B25" s="61"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="6"/>
+      <c r="AK24" s="5"/>
+      <c r="AL24" s="6"/>
+      <c r="AM24" s="5"/>
+      <c r="AN24" s="6"/>
+      <c r="AO24" s="5"/>
+      <c r="AP24" s="16"/>
+    </row>
+    <row r="25" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B25" s="69"/>
       <c r="C25" s="15"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
@@ -3485,9 +3859,17 @@
       <c r="AF25" s="6"/>
       <c r="AG25" s="5"/>
       <c r="AH25" s="16"/>
-    </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B26" s="61"/>
+      <c r="AI25" s="15"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="6"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="5"/>
+      <c r="AP25" s="16"/>
+    </row>
+    <row r="26" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B26" s="69"/>
       <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
@@ -3528,9 +3910,17 @@
       <c r="AF26" s="6"/>
       <c r="AG26" s="5"/>
       <c r="AH26" s="16"/>
-    </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B27" s="61"/>
+      <c r="AI26" s="15"/>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="6"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="16"/>
+    </row>
+    <row r="27" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B27" s="69"/>
       <c r="C27" s="15"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
@@ -3571,9 +3961,17 @@
       <c r="AF27" s="6"/>
       <c r="AG27" s="5"/>
       <c r="AH27" s="16"/>
-    </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B28" s="61"/>
+      <c r="AI27" s="15"/>
+      <c r="AJ27" s="6"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="6"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="6"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="16"/>
+    </row>
+    <row r="28" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B28" s="69"/>
       <c r="C28" s="15"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
@@ -3614,9 +4012,17 @@
       <c r="AF28" s="6"/>
       <c r="AG28" s="5"/>
       <c r="AH28" s="16"/>
-    </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B29" s="61"/>
+      <c r="AI28" s="15"/>
+      <c r="AJ28" s="6"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="6"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="6"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="16"/>
+    </row>
+    <row r="29" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B29" s="69"/>
       <c r="C29" s="15"/>
       <c r="D29" s="6"/>
       <c r="E29" s="5"/>
@@ -3657,9 +4063,17 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="5"/>
       <c r="AH29" s="16"/>
-    </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B30" s="61"/>
+      <c r="AI29" s="15"/>
+      <c r="AJ29" s="6"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="6"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="6"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="16"/>
+    </row>
+    <row r="30" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B30" s="69"/>
       <c r="C30" s="15"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
@@ -3700,9 +4114,17 @@
       <c r="AF30" s="6"/>
       <c r="AG30" s="5"/>
       <c r="AH30" s="16"/>
-    </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B31" s="61"/>
+      <c r="AI30" s="15"/>
+      <c r="AJ30" s="6"/>
+      <c r="AK30" s="5"/>
+      <c r="AL30" s="6"/>
+      <c r="AM30" s="5"/>
+      <c r="AN30" s="6"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="16"/>
+    </row>
+    <row r="31" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B31" s="69"/>
       <c r="C31" s="15"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
@@ -3743,9 +4165,17 @@
       <c r="AF31" s="6"/>
       <c r="AG31" s="5"/>
       <c r="AH31" s="16"/>
-    </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B32" s="61"/>
+      <c r="AI31" s="15"/>
+      <c r="AJ31" s="6"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="6"/>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="6"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="16"/>
+    </row>
+    <row r="32" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B32" s="69"/>
       <c r="C32" s="15"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
@@ -3786,9 +4216,17 @@
       <c r="AF32" s="6"/>
       <c r="AG32" s="5"/>
       <c r="AH32" s="16"/>
-    </row>
-    <row r="33" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B33" s="61"/>
+      <c r="AI32" s="15"/>
+      <c r="AJ32" s="6"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="6"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="6"/>
+      <c r="AO32" s="5"/>
+      <c r="AP32" s="16"/>
+    </row>
+    <row r="33" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B33" s="69"/>
       <c r="C33" s="15"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
@@ -3829,9 +4267,17 @@
       <c r="AF33" s="6"/>
       <c r="AG33" s="5"/>
       <c r="AH33" s="16"/>
-    </row>
-    <row r="34" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B34" s="61"/>
+      <c r="AI33" s="15"/>
+      <c r="AJ33" s="6"/>
+      <c r="AK33" s="5"/>
+      <c r="AL33" s="6"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="6"/>
+      <c r="AO33" s="5"/>
+      <c r="AP33" s="16"/>
+    </row>
+    <row r="34" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B34" s="69"/>
       <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
@@ -3872,9 +4318,17 @@
       <c r="AF34" s="6"/>
       <c r="AG34" s="5"/>
       <c r="AH34" s="16"/>
-    </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B35" s="61"/>
+      <c r="AI34" s="15"/>
+      <c r="AJ34" s="6"/>
+      <c r="AK34" s="5"/>
+      <c r="AL34" s="6"/>
+      <c r="AM34" s="5"/>
+      <c r="AN34" s="6"/>
+      <c r="AO34" s="5"/>
+      <c r="AP34" s="16"/>
+    </row>
+    <row r="35" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B35" s="69"/>
       <c r="C35" s="15"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
@@ -3915,9 +4369,17 @@
       <c r="AF35" s="6"/>
       <c r="AG35" s="5"/>
       <c r="AH35" s="16"/>
-    </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B36" s="63"/>
+      <c r="AI35" s="15"/>
+      <c r="AJ35" s="6"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="6"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="6"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="16"/>
+    </row>
+    <row r="36" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B36" s="71"/>
       <c r="C36" s="17"/>
       <c r="D36" s="8"/>
       <c r="E36" s="7"/>
@@ -3958,110 +4420,142 @@
       <c r="AF36" s="8"/>
       <c r="AG36" s="7"/>
       <c r="AH36" s="18"/>
-    </row>
-    <row r="37" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B37" s="60" t="s">
+      <c r="AI36" s="17"/>
+      <c r="AJ36" s="8"/>
+      <c r="AK36" s="7"/>
+      <c r="AL36" s="8"/>
+      <c r="AM36" s="7"/>
+      <c r="AN36" s="8"/>
+      <c r="AO36" s="7"/>
+      <c r="AP36" s="18"/>
+    </row>
+    <row r="37" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B37" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="43" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="46" t="s">
+      <c r="E37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="F37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="46" t="s">
+      <c r="G37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="H37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="46" t="s">
+      <c r="I37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="J37" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K37" s="45" t="s">
+      <c r="K37" s="43" t="s">
         <v>41</v>
       </c>
       <c r="L37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M37" s="46" t="s">
+      <c r="M37" s="44" t="s">
         <v>42</v>
       </c>
       <c r="N37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O37" s="46" t="s">
+      <c r="O37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="P37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q37" s="46" t="s">
+      <c r="Q37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="R37" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="S37" s="45" t="s">
+      <c r="S37" s="43" t="s">
         <v>41</v>
       </c>
       <c r="T37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="U37" s="46" t="s">
+      <c r="U37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="V37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="W37" s="46" t="s">
+      <c r="W37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="X37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Y37" s="46" t="s">
+      <c r="Y37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="Z37" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AA37" s="45" t="s">
+      <c r="AA37" s="43" t="s">
         <v>41</v>
       </c>
       <c r="AB37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AC37" s="46" t="s">
+      <c r="AC37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="AD37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AE37" s="46" t="s">
+      <c r="AE37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="AF37" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AG37" s="46" t="s">
+      <c r="AG37" s="44" t="s">
         <v>41</v>
       </c>
       <c r="AH37" s="35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B38" s="61"/>
+      <c r="AI37" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ37" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK37" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL37" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM37" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN37" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO37" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP37" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B38" s="69"/>
       <c r="C38" s="30">
         <v>0.25</v>
       </c>
@@ -4134,9 +4628,33 @@
       <c r="AF38" s="31"/>
       <c r="AG38" s="32"/>
       <c r="AH38" s="33"/>
-    </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B39" s="61"/>
+      <c r="AI38" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ38" s="31">
+        <v>1</v>
+      </c>
+      <c r="AK38" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="AL38" s="31">
+        <v>1</v>
+      </c>
+      <c r="AM38" s="32">
+        <v>0</v>
+      </c>
+      <c r="AN38" s="31">
+        <v>0</v>
+      </c>
+      <c r="AO38" s="32">
+        <v>0</v>
+      </c>
+      <c r="AP38" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B39" s="69"/>
       <c r="C39" s="15">
         <v>0.45</v>
       </c>
@@ -4209,9 +4727,33 @@
       <c r="AF39" s="6"/>
       <c r="AG39" s="5"/>
       <c r="AH39" s="16"/>
-    </row>
-    <row r="40" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B40" s="61"/>
+      <c r="AI39" s="15">
+        <v>100</v>
+      </c>
+      <c r="AJ39" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK39" s="5">
+        <v>100</v>
+      </c>
+      <c r="AL39" s="6">
+        <v>1</v>
+      </c>
+      <c r="AM39" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AN39" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO39" s="5">
+        <v>100</v>
+      </c>
+      <c r="AP39" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B40" s="69"/>
       <c r="C40" s="15">
         <v>0.65</v>
       </c>
@@ -4284,9 +4826,21 @@
       <c r="AF40" s="6"/>
       <c r="AG40" s="5"/>
       <c r="AH40" s="16"/>
-    </row>
-    <row r="41" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B41" s="61"/>
+      <c r="AI40" s="15"/>
+      <c r="AJ40" s="6"/>
+      <c r="AK40" s="5"/>
+      <c r="AL40" s="6"/>
+      <c r="AM40" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AN40" s="6">
+        <v>1</v>
+      </c>
+      <c r="AO40" s="5"/>
+      <c r="AP40" s="16"/>
+    </row>
+    <row r="41" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B41" s="69"/>
       <c r="C41" s="15">
         <v>0.75</v>
       </c>
@@ -4351,9 +4905,21 @@
       <c r="AF41" s="6"/>
       <c r="AG41" s="5"/>
       <c r="AH41" s="16"/>
-    </row>
-    <row r="42" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B42" s="61"/>
+      <c r="AI41" s="15"/>
+      <c r="AJ41" s="6"/>
+      <c r="AK41" s="5"/>
+      <c r="AL41" s="6"/>
+      <c r="AM41" s="5">
+        <v>100</v>
+      </c>
+      <c r="AN41" s="6">
+        <v>1</v>
+      </c>
+      <c r="AO41" s="5"/>
+      <c r="AP41" s="16"/>
+    </row>
+    <row r="42" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B42" s="69"/>
       <c r="C42" s="15">
         <v>0.95</v>
       </c>
@@ -4418,9 +4984,17 @@
       <c r="AF42" s="6"/>
       <c r="AG42" s="5"/>
       <c r="AH42" s="16"/>
-    </row>
-    <row r="43" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B43" s="61"/>
+      <c r="AI42" s="15"/>
+      <c r="AJ42" s="6"/>
+      <c r="AK42" s="5"/>
+      <c r="AL42" s="6"/>
+      <c r="AM42" s="5"/>
+      <c r="AN42" s="6"/>
+      <c r="AO42" s="5"/>
+      <c r="AP42" s="16"/>
+    </row>
+    <row r="43" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B43" s="69"/>
       <c r="C43" s="15">
         <v>2</v>
       </c>
@@ -4481,9 +5055,17 @@
       <c r="AF43" s="6"/>
       <c r="AG43" s="5"/>
       <c r="AH43" s="16"/>
-    </row>
-    <row r="44" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B44" s="61"/>
+      <c r="AI43" s="15"/>
+      <c r="AJ43" s="6"/>
+      <c r="AK43" s="5"/>
+      <c r="AL43" s="6"/>
+      <c r="AM43" s="5"/>
+      <c r="AN43" s="6"/>
+      <c r="AO43" s="5"/>
+      <c r="AP43" s="16"/>
+    </row>
+    <row r="44" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B44" s="69"/>
       <c r="C44" s="15">
         <v>3</v>
       </c>
@@ -4536,9 +5118,17 @@
       <c r="AF44" s="6"/>
       <c r="AG44" s="5"/>
       <c r="AH44" s="16"/>
-    </row>
-    <row r="45" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B45" s="61"/>
+      <c r="AI44" s="15"/>
+      <c r="AJ44" s="6"/>
+      <c r="AK44" s="5"/>
+      <c r="AL44" s="6"/>
+      <c r="AM44" s="5"/>
+      <c r="AN44" s="6"/>
+      <c r="AO44" s="5"/>
+      <c r="AP44" s="16"/>
+    </row>
+    <row r="45" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B45" s="69"/>
       <c r="C45" s="15">
         <v>4.8</v>
       </c>
@@ -4591,9 +5181,17 @@
       <c r="AF45" s="6"/>
       <c r="AG45" s="5"/>
       <c r="AH45" s="16"/>
-    </row>
-    <row r="46" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B46" s="61"/>
+      <c r="AI45" s="15"/>
+      <c r="AJ45" s="6"/>
+      <c r="AK45" s="5"/>
+      <c r="AL45" s="6"/>
+      <c r="AM45" s="5"/>
+      <c r="AN45" s="6"/>
+      <c r="AO45" s="5"/>
+      <c r="AP45" s="16"/>
+    </row>
+    <row r="46" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B46" s="69"/>
       <c r="C46" s="15">
         <v>7.8</v>
       </c>
@@ -4642,9 +5240,17 @@
       <c r="AF46" s="6"/>
       <c r="AG46" s="5"/>
       <c r="AH46" s="16"/>
-    </row>
-    <row r="47" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B47" s="61"/>
+      <c r="AI46" s="15"/>
+      <c r="AJ46" s="6"/>
+      <c r="AK46" s="5"/>
+      <c r="AL46" s="6"/>
+      <c r="AM46" s="5"/>
+      <c r="AN46" s="6"/>
+      <c r="AO46" s="5"/>
+      <c r="AP46" s="16"/>
+    </row>
+    <row r="47" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B47" s="69"/>
       <c r="C47" s="15">
         <v>7.9</v>
       </c>
@@ -4693,9 +5299,17 @@
       <c r="AF47" s="6"/>
       <c r="AG47" s="5"/>
       <c r="AH47" s="16"/>
-    </row>
-    <row r="48" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B48" s="61"/>
+      <c r="AI47" s="15"/>
+      <c r="AJ47" s="6"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="6"/>
+      <c r="AM47" s="5"/>
+      <c r="AN47" s="6"/>
+      <c r="AO47" s="5"/>
+      <c r="AP47" s="16"/>
+    </row>
+    <row r="48" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B48" s="69"/>
       <c r="C48" s="15"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5">
@@ -4736,9 +5350,17 @@
       <c r="AF48" s="6"/>
       <c r="AG48" s="5"/>
       <c r="AH48" s="16"/>
-    </row>
-    <row r="49" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B49" s="61"/>
+      <c r="AI48" s="15"/>
+      <c r="AJ48" s="6"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="6"/>
+      <c r="AM48" s="5"/>
+      <c r="AN48" s="6"/>
+      <c r="AO48" s="5"/>
+      <c r="AP48" s="16"/>
+    </row>
+    <row r="49" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B49" s="69"/>
       <c r="C49" s="15"/>
       <c r="D49" s="6"/>
       <c r="E49" s="5">
@@ -4779,9 +5401,17 @@
       <c r="AF49" s="6"/>
       <c r="AG49" s="5"/>
       <c r="AH49" s="16"/>
-    </row>
-    <row r="50" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B50" s="61"/>
+      <c r="AI49" s="15"/>
+      <c r="AJ49" s="6"/>
+      <c r="AK49" s="5"/>
+      <c r="AL49" s="6"/>
+      <c r="AM49" s="5"/>
+      <c r="AN49" s="6"/>
+      <c r="AO49" s="5"/>
+      <c r="AP49" s="16"/>
+    </row>
+    <row r="50" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B50" s="69"/>
       <c r="C50" s="15"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5">
@@ -4822,9 +5452,17 @@
       <c r="AF50" s="6"/>
       <c r="AG50" s="5"/>
       <c r="AH50" s="16"/>
-    </row>
-    <row r="51" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B51" s="61"/>
+      <c r="AI50" s="15"/>
+      <c r="AJ50" s="6"/>
+      <c r="AK50" s="5"/>
+      <c r="AL50" s="6"/>
+      <c r="AM50" s="5"/>
+      <c r="AN50" s="6"/>
+      <c r="AO50" s="5"/>
+      <c r="AP50" s="16"/>
+    </row>
+    <row r="51" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B51" s="69"/>
       <c r="C51" s="15"/>
       <c r="D51" s="6"/>
       <c r="E51" s="5">
@@ -4865,9 +5503,17 @@
       <c r="AF51" s="6"/>
       <c r="AG51" s="5"/>
       <c r="AH51" s="16"/>
-    </row>
-    <row r="52" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B52" s="61"/>
+      <c r="AI51" s="15"/>
+      <c r="AJ51" s="6"/>
+      <c r="AK51" s="5"/>
+      <c r="AL51" s="6"/>
+      <c r="AM51" s="5"/>
+      <c r="AN51" s="6"/>
+      <c r="AO51" s="5"/>
+      <c r="AP51" s="16"/>
+    </row>
+    <row r="52" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B52" s="69"/>
       <c r="C52" s="15"/>
       <c r="D52" s="6"/>
       <c r="E52" s="5">
@@ -4908,9 +5554,17 @@
       <c r="AF52" s="6"/>
       <c r="AG52" s="5"/>
       <c r="AH52" s="16"/>
-    </row>
-    <row r="53" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B53" s="61"/>
+      <c r="AI52" s="15"/>
+      <c r="AJ52" s="6"/>
+      <c r="AK52" s="5"/>
+      <c r="AL52" s="6"/>
+      <c r="AM52" s="5"/>
+      <c r="AN52" s="6"/>
+      <c r="AO52" s="5"/>
+      <c r="AP52" s="16"/>
+    </row>
+    <row r="53" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B53" s="69"/>
       <c r="C53" s="15"/>
       <c r="D53" s="6"/>
       <c r="E53" s="5">
@@ -4951,9 +5605,17 @@
       <c r="AF53" s="6"/>
       <c r="AG53" s="5"/>
       <c r="AH53" s="16"/>
-    </row>
-    <row r="54" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B54" s="61"/>
+      <c r="AI53" s="15"/>
+      <c r="AJ53" s="6"/>
+      <c r="AK53" s="5"/>
+      <c r="AL53" s="6"/>
+      <c r="AM53" s="5"/>
+      <c r="AN53" s="6"/>
+      <c r="AO53" s="5"/>
+      <c r="AP53" s="16"/>
+    </row>
+    <row r="54" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B54" s="69"/>
       <c r="C54" s="15"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5">
@@ -4990,9 +5652,17 @@
       <c r="AF54" s="6"/>
       <c r="AG54" s="5"/>
       <c r="AH54" s="16"/>
-    </row>
-    <row r="55" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B55" s="61"/>
+      <c r="AI54" s="15"/>
+      <c r="AJ54" s="6"/>
+      <c r="AK54" s="5"/>
+      <c r="AL54" s="6"/>
+      <c r="AM54" s="5"/>
+      <c r="AN54" s="6"/>
+      <c r="AO54" s="5"/>
+      <c r="AP54" s="16"/>
+    </row>
+    <row r="55" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B55" s="69"/>
       <c r="C55" s="15"/>
       <c r="D55" s="6"/>
       <c r="E55" s="5">
@@ -5029,9 +5699,17 @@
       <c r="AF55" s="6"/>
       <c r="AG55" s="5"/>
       <c r="AH55" s="16"/>
-    </row>
-    <row r="56" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B56" s="61"/>
+      <c r="AI55" s="15"/>
+      <c r="AJ55" s="6"/>
+      <c r="AK55" s="5"/>
+      <c r="AL55" s="6"/>
+      <c r="AM55" s="5"/>
+      <c r="AN55" s="6"/>
+      <c r="AO55" s="5"/>
+      <c r="AP55" s="16"/>
+    </row>
+    <row r="56" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B56" s="69"/>
       <c r="C56" s="15"/>
       <c r="D56" s="6"/>
       <c r="E56" s="5">
@@ -5068,9 +5746,17 @@
       <c r="AF56" s="6"/>
       <c r="AG56" s="5"/>
       <c r="AH56" s="16"/>
-    </row>
-    <row r="57" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B57" s="61"/>
+      <c r="AI56" s="15"/>
+      <c r="AJ56" s="6"/>
+      <c r="AK56" s="5"/>
+      <c r="AL56" s="6"/>
+      <c r="AM56" s="5"/>
+      <c r="AN56" s="6"/>
+      <c r="AO56" s="5"/>
+      <c r="AP56" s="16"/>
+    </row>
+    <row r="57" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B57" s="69"/>
       <c r="C57" s="15"/>
       <c r="D57" s="6"/>
       <c r="E57" s="5">
@@ -5107,9 +5793,17 @@
       <c r="AF57" s="6"/>
       <c r="AG57" s="5"/>
       <c r="AH57" s="16"/>
-    </row>
-    <row r="58" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B58" s="61"/>
+      <c r="AI57" s="15"/>
+      <c r="AJ57" s="6"/>
+      <c r="AK57" s="5"/>
+      <c r="AL57" s="6"/>
+      <c r="AM57" s="5"/>
+      <c r="AN57" s="6"/>
+      <c r="AO57" s="5"/>
+      <c r="AP57" s="16"/>
+    </row>
+    <row r="58" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B58" s="69"/>
       <c r="C58" s="15"/>
       <c r="D58" s="6"/>
       <c r="E58" s="5">
@@ -5146,9 +5840,17 @@
       <c r="AF58" s="6"/>
       <c r="AG58" s="5"/>
       <c r="AH58" s="16"/>
-    </row>
-    <row r="59" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B59" s="61"/>
+      <c r="AI58" s="15"/>
+      <c r="AJ58" s="6"/>
+      <c r="AK58" s="5"/>
+      <c r="AL58" s="6"/>
+      <c r="AM58" s="5"/>
+      <c r="AN58" s="6"/>
+      <c r="AO58" s="5"/>
+      <c r="AP58" s="16"/>
+    </row>
+    <row r="59" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B59" s="69"/>
       <c r="C59" s="15"/>
       <c r="D59" s="6"/>
       <c r="E59" s="5">
@@ -5185,9 +5887,17 @@
       <c r="AF59" s="6"/>
       <c r="AG59" s="5"/>
       <c r="AH59" s="16"/>
-    </row>
-    <row r="60" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B60" s="61"/>
+      <c r="AI59" s="15"/>
+      <c r="AJ59" s="6"/>
+      <c r="AK59" s="5"/>
+      <c r="AL59" s="6"/>
+      <c r="AM59" s="5"/>
+      <c r="AN59" s="6"/>
+      <c r="AO59" s="5"/>
+      <c r="AP59" s="16"/>
+    </row>
+    <row r="60" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B60" s="69"/>
       <c r="C60" s="15"/>
       <c r="D60" s="6"/>
       <c r="E60" s="5">
@@ -5224,9 +5934,17 @@
       <c r="AF60" s="6"/>
       <c r="AG60" s="5"/>
       <c r="AH60" s="16"/>
-    </row>
-    <row r="61" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B61" s="61"/>
+      <c r="AI60" s="15"/>
+      <c r="AJ60" s="6"/>
+      <c r="AK60" s="5"/>
+      <c r="AL60" s="6"/>
+      <c r="AM60" s="5"/>
+      <c r="AN60" s="6"/>
+      <c r="AO60" s="5"/>
+      <c r="AP60" s="16"/>
+    </row>
+    <row r="61" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B61" s="69"/>
       <c r="C61" s="15"/>
       <c r="D61" s="6"/>
       <c r="E61" s="5">
@@ -5263,9 +5981,17 @@
       <c r="AF61" s="6"/>
       <c r="AG61" s="5"/>
       <c r="AH61" s="16"/>
-    </row>
-    <row r="62" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B62" s="61"/>
+      <c r="AI61" s="15"/>
+      <c r="AJ61" s="6"/>
+      <c r="AK61" s="5"/>
+      <c r="AL61" s="6"/>
+      <c r="AM61" s="5"/>
+      <c r="AN61" s="6"/>
+      <c r="AO61" s="5"/>
+      <c r="AP61" s="16"/>
+    </row>
+    <row r="62" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B62" s="69"/>
       <c r="C62" s="15"/>
       <c r="D62" s="6"/>
       <c r="E62" s="5">
@@ -5302,9 +6028,17 @@
       <c r="AF62" s="6"/>
       <c r="AG62" s="5"/>
       <c r="AH62" s="16"/>
-    </row>
-    <row r="63" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B63" s="61"/>
+      <c r="AI62" s="15"/>
+      <c r="AJ62" s="6"/>
+      <c r="AK62" s="5"/>
+      <c r="AL62" s="6"/>
+      <c r="AM62" s="5"/>
+      <c r="AN62" s="6"/>
+      <c r="AO62" s="5"/>
+      <c r="AP62" s="16"/>
+    </row>
+    <row r="63" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B63" s="69"/>
       <c r="C63" s="15"/>
       <c r="D63" s="6"/>
       <c r="E63" s="5">
@@ -5341,9 +6075,17 @@
       <c r="AF63" s="6"/>
       <c r="AG63" s="5"/>
       <c r="AH63" s="16"/>
-    </row>
-    <row r="64" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B64" s="61"/>
+      <c r="AI63" s="15"/>
+      <c r="AJ63" s="6"/>
+      <c r="AK63" s="5"/>
+      <c r="AL63" s="6"/>
+      <c r="AM63" s="5"/>
+      <c r="AN63" s="6"/>
+      <c r="AO63" s="5"/>
+      <c r="AP63" s="16"/>
+    </row>
+    <row r="64" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B64" s="69"/>
       <c r="C64" s="15"/>
       <c r="D64" s="6"/>
       <c r="E64" s="5">
@@ -5380,9 +6122,17 @@
       <c r="AF64" s="6"/>
       <c r="AG64" s="5"/>
       <c r="AH64" s="16"/>
-    </row>
-    <row r="65" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B65" s="61"/>
+      <c r="AI64" s="15"/>
+      <c r="AJ64" s="6"/>
+      <c r="AK64" s="5"/>
+      <c r="AL64" s="6"/>
+      <c r="AM64" s="5"/>
+      <c r="AN64" s="6"/>
+      <c r="AO64" s="5"/>
+      <c r="AP64" s="16"/>
+    </row>
+    <row r="65" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B65" s="69"/>
       <c r="C65" s="15"/>
       <c r="D65" s="6"/>
       <c r="E65" s="5">
@@ -5419,9 +6169,17 @@
       <c r="AF65" s="6"/>
       <c r="AG65" s="5"/>
       <c r="AH65" s="16"/>
-    </row>
-    <row r="66" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B66" s="61"/>
+      <c r="AI65" s="15"/>
+      <c r="AJ65" s="6"/>
+      <c r="AK65" s="5"/>
+      <c r="AL65" s="6"/>
+      <c r="AM65" s="5"/>
+      <c r="AN65" s="6"/>
+      <c r="AO65" s="5"/>
+      <c r="AP65" s="16"/>
+    </row>
+    <row r="66" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B66" s="69"/>
       <c r="C66" s="15"/>
       <c r="D66" s="6"/>
       <c r="E66" s="5">
@@ -5458,9 +6216,17 @@
       <c r="AF66" s="6"/>
       <c r="AG66" s="5"/>
       <c r="AH66" s="16"/>
-    </row>
-    <row r="67" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B67" s="61"/>
+      <c r="AI66" s="15"/>
+      <c r="AJ66" s="6"/>
+      <c r="AK66" s="5"/>
+      <c r="AL66" s="6"/>
+      <c r="AM66" s="5"/>
+      <c r="AN66" s="6"/>
+      <c r="AO66" s="5"/>
+      <c r="AP66" s="16"/>
+    </row>
+    <row r="67" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B67" s="69"/>
       <c r="C67" s="15"/>
       <c r="D67" s="6"/>
       <c r="E67" s="5">
@@ -5497,9 +6263,17 @@
       <c r="AF67" s="6"/>
       <c r="AG67" s="5"/>
       <c r="AH67" s="16"/>
-    </row>
-    <row r="68" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B68" s="61"/>
+      <c r="AI67" s="15"/>
+      <c r="AJ67" s="6"/>
+      <c r="AK67" s="5"/>
+      <c r="AL67" s="6"/>
+      <c r="AM67" s="5"/>
+      <c r="AN67" s="6"/>
+      <c r="AO67" s="5"/>
+      <c r="AP67" s="16"/>
+    </row>
+    <row r="68" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B68" s="69"/>
       <c r="C68" s="15"/>
       <c r="D68" s="6"/>
       <c r="E68" s="5">
@@ -5536,9 +6310,17 @@
       <c r="AF68" s="6"/>
       <c r="AG68" s="5"/>
       <c r="AH68" s="16"/>
-    </row>
-    <row r="69" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B69" s="61"/>
+      <c r="AI68" s="15"/>
+      <c r="AJ68" s="6"/>
+      <c r="AK68" s="5"/>
+      <c r="AL68" s="6"/>
+      <c r="AM68" s="5"/>
+      <c r="AN68" s="6"/>
+      <c r="AO68" s="5"/>
+      <c r="AP68" s="16"/>
+    </row>
+    <row r="69" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B69" s="69"/>
       <c r="C69" s="15"/>
       <c r="D69" s="6"/>
       <c r="E69" s="5">
@@ -5575,9 +6357,17 @@
       <c r="AF69" s="6"/>
       <c r="AG69" s="5"/>
       <c r="AH69" s="16"/>
-    </row>
-    <row r="70" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B70" s="63"/>
+      <c r="AI69" s="15"/>
+      <c r="AJ69" s="6"/>
+      <c r="AK69" s="5"/>
+      <c r="AL69" s="6"/>
+      <c r="AM69" s="5"/>
+      <c r="AN69" s="6"/>
+      <c r="AO69" s="5"/>
+      <c r="AP69" s="16"/>
+    </row>
+    <row r="70" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B70" s="71"/>
       <c r="C70" s="17"/>
       <c r="D70" s="8"/>
       <c r="E70" s="7">
@@ -5614,110 +6404,142 @@
       <c r="AF70" s="8"/>
       <c r="AG70" s="7"/>
       <c r="AH70" s="18"/>
-    </row>
-    <row r="71" spans="2:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="60" t="s">
+      <c r="AI70" s="17"/>
+      <c r="AJ70" s="8"/>
+      <c r="AK70" s="7"/>
+      <c r="AL70" s="8"/>
+      <c r="AM70" s="7"/>
+      <c r="AN70" s="8"/>
+      <c r="AO70" s="7"/>
+      <c r="AP70" s="18"/>
+    </row>
+    <row r="71" spans="2:42" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="C71" s="45" t="s">
+      <c r="C71" s="43" t="s">
         <v>47</v>
       </c>
       <c r="D71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="46" t="s">
+      <c r="E71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="F71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G71" s="46" t="s">
+      <c r="G71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="H71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I71" s="46" t="s">
+      <c r="I71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="J71" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K71" s="45" t="s">
+      <c r="K71" s="43" t="s">
         <v>47</v>
       </c>
       <c r="L71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M71" s="46" t="s">
+      <c r="M71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="N71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O71" s="46" t="s">
+      <c r="O71" s="44" t="s">
         <v>48</v>
       </c>
       <c r="P71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q71" s="46" t="s">
+      <c r="Q71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="R71" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="S71" s="45" t="s">
+      <c r="S71" s="43" t="s">
         <v>47</v>
       </c>
       <c r="T71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="U71" s="46" t="s">
+      <c r="U71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="V71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="W71" s="46" t="s">
+      <c r="W71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="X71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Y71" s="46" t="s">
+      <c r="Y71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="Z71" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AA71" s="45" t="s">
+      <c r="AA71" s="43" t="s">
         <v>47</v>
       </c>
       <c r="AB71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AC71" s="46" t="s">
+      <c r="AC71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="AD71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AE71" s="46" t="s">
+      <c r="AE71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="AF71" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AG71" s="46" t="s">
+      <c r="AG71" s="44" t="s">
         <v>47</v>
       </c>
       <c r="AH71" s="35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="72" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B72" s="61"/>
+      <c r="AI71" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ71" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK71" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL71" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM71" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN71" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO71" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP71" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B72" s="69"/>
       <c r="C72" s="30">
         <v>0.10170583333333333</v>
       </c>
@@ -5778,9 +6600,33 @@
       <c r="AF72" s="31"/>
       <c r="AG72" s="32"/>
       <c r="AH72" s="33"/>
-    </row>
-    <row r="73" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B73" s="61"/>
+      <c r="AI72" s="30">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AJ72" s="31">
+        <v>1</v>
+      </c>
+      <c r="AK72" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AL72" s="31">
+        <v>1</v>
+      </c>
+      <c r="AM72" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AN72" s="31">
+        <v>1</v>
+      </c>
+      <c r="AO72" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AP72" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B73" s="69"/>
       <c r="C73" s="15">
         <v>0.10498666666666666</v>
       </c>
@@ -5841,9 +6687,33 @@
       <c r="AF73" s="6"/>
       <c r="AG73" s="5"/>
       <c r="AH73" s="16"/>
-    </row>
-    <row r="74" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B74" s="61"/>
+      <c r="AI73" s="15">
+        <v>100</v>
+      </c>
+      <c r="AJ73" s="6">
+        <v>1</v>
+      </c>
+      <c r="AK73" s="5">
+        <v>100</v>
+      </c>
+      <c r="AL73" s="6">
+        <v>1</v>
+      </c>
+      <c r="AM73" s="5">
+        <v>100</v>
+      </c>
+      <c r="AN73" s="6">
+        <v>1</v>
+      </c>
+      <c r="AO73" s="5">
+        <v>100</v>
+      </c>
+      <c r="AP73" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B74" s="69"/>
       <c r="C74" s="15">
         <v>0.63976250000000001</v>
       </c>
@@ -5904,9 +6774,17 @@
       <c r="AF74" s="6"/>
       <c r="AG74" s="5"/>
       <c r="AH74" s="16"/>
-    </row>
-    <row r="75" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B75" s="61"/>
+      <c r="AI74" s="15"/>
+      <c r="AJ74" s="6"/>
+      <c r="AK74" s="5"/>
+      <c r="AL74" s="6"/>
+      <c r="AM74" s="5"/>
+      <c r="AN74" s="6"/>
+      <c r="AO74" s="5"/>
+      <c r="AP74" s="16"/>
+    </row>
+    <row r="75" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B75" s="69"/>
       <c r="C75" s="15">
         <v>0.6430433333333333</v>
       </c>
@@ -5967,9 +6845,17 @@
       <c r="AF75" s="6"/>
       <c r="AG75" s="5"/>
       <c r="AH75" s="16"/>
-    </row>
-    <row r="76" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B76" s="61"/>
+      <c r="AI75" s="15"/>
+      <c r="AJ75" s="6"/>
+      <c r="AK75" s="5"/>
+      <c r="AL75" s="6"/>
+      <c r="AM75" s="5"/>
+      <c r="AN75" s="6"/>
+      <c r="AO75" s="5"/>
+      <c r="AP75" s="16"/>
+    </row>
+    <row r="76" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B76" s="69"/>
       <c r="C76" s="15"/>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -6018,9 +6904,17 @@
       <c r="AF76" s="6"/>
       <c r="AG76" s="5"/>
       <c r="AH76" s="16"/>
-    </row>
-    <row r="77" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B77" s="62"/>
+      <c r="AI76" s="15"/>
+      <c r="AJ76" s="6"/>
+      <c r="AK76" s="5"/>
+      <c r="AL76" s="6"/>
+      <c r="AM76" s="5"/>
+      <c r="AN76" s="6"/>
+      <c r="AO76" s="5"/>
+      <c r="AP76" s="16"/>
+    </row>
+    <row r="77" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B77" s="70"/>
       <c r="C77" s="28"/>
       <c r="D77" s="10"/>
       <c r="E77" s="9"/>
@@ -6065,9 +6959,17 @@
       <c r="AF77" s="10"/>
       <c r="AG77" s="9"/>
       <c r="AH77" s="29"/>
-    </row>
-    <row r="78" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B78" s="62"/>
+      <c r="AI77" s="28"/>
+      <c r="AJ77" s="10"/>
+      <c r="AK77" s="9"/>
+      <c r="AL77" s="10"/>
+      <c r="AM77" s="9"/>
+      <c r="AN77" s="10"/>
+      <c r="AO77" s="9"/>
+      <c r="AP77" s="29"/>
+    </row>
+    <row r="78" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B78" s="70"/>
       <c r="C78" s="28"/>
       <c r="D78" s="10"/>
       <c r="E78" s="9"/>
@@ -6108,9 +7010,17 @@
       <c r="AF78" s="10"/>
       <c r="AG78" s="9"/>
       <c r="AH78" s="29"/>
-    </row>
-    <row r="79" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="B79" s="63"/>
+      <c r="AI78" s="28"/>
+      <c r="AJ78" s="10"/>
+      <c r="AK78" s="9"/>
+      <c r="AL78" s="10"/>
+      <c r="AM78" s="9"/>
+      <c r="AN78" s="10"/>
+      <c r="AO78" s="9"/>
+      <c r="AP78" s="29"/>
+    </row>
+    <row r="79" spans="2:42" x14ac:dyDescent="0.3">
+      <c r="B79" s="71"/>
       <c r="C79" s="17"/>
       <c r="D79" s="8"/>
       <c r="E79" s="7"/>
@@ -6151,109 +7061,141 @@
       <c r="AF79" s="8"/>
       <c r="AG79" s="7"/>
       <c r="AH79" s="18"/>
-    </row>
-    <row r="80" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI79" s="17"/>
+      <c r="AJ79" s="8"/>
+      <c r="AK79" s="7"/>
+      <c r="AL79" s="8"/>
+      <c r="AM79" s="7"/>
+      <c r="AN79" s="8"/>
+      <c r="AO79" s="7"/>
+      <c r="AP79" s="18"/>
+    </row>
+    <row r="80" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B80" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C80" s="45" t="s">
+      <c r="C80" s="43" t="s">
         <v>49</v>
       </c>
       <c r="D80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E80" s="46" t="s">
+      <c r="E80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="F80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G80" s="46" t="s">
+      <c r="G80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="H80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I80" s="46" t="s">
+      <c r="I80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="J80" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K80" s="45" t="s">
+      <c r="K80" s="43" t="s">
         <v>49</v>
       </c>
       <c r="L80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M80" s="46" t="s">
+      <c r="M80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="N80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O80" s="46" t="s">
+      <c r="O80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="P80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q80" s="46" t="s">
+      <c r="Q80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="R80" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="S80" s="45" t="s">
+      <c r="S80" s="43" t="s">
         <v>49</v>
       </c>
       <c r="T80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="U80" s="46" t="s">
+      <c r="U80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="V80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="W80" s="46" t="s">
+      <c r="W80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="X80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Y80" s="46" t="s">
+      <c r="Y80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="Z80" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AA80" s="45" t="s">
+      <c r="AA80" s="43" t="s">
         <v>49</v>
       </c>
       <c r="AB80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AC80" s="46" t="s">
+      <c r="AC80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="AD80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AE80" s="46" t="s">
+      <c r="AE80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="AF80" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AG80" s="46" t="s">
+      <c r="AG80" s="44" t="s">
         <v>49</v>
       </c>
       <c r="AH80" s="35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI80" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ80" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK80" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL80" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM80" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN80" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO80" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP80" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B81" s="25" t="s">
         <v>19</v>
       </c>
@@ -6305,8 +7247,32 @@
       <c r="AF81" s="31"/>
       <c r="AG81" s="32"/>
       <c r="AH81" s="33"/>
-    </row>
-    <row r="82" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI81" s="30">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AJ81" s="31">
+        <v>1</v>
+      </c>
+      <c r="AK81" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AL81" s="31">
+        <v>1</v>
+      </c>
+      <c r="AM81" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AN81" s="31">
+        <v>1</v>
+      </c>
+      <c r="AO81" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AP81" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B82" s="26" t="s">
         <v>20</v>
       </c>
@@ -6358,109 +7324,157 @@
       <c r="AF82" s="8"/>
       <c r="AG82" s="7"/>
       <c r="AH82" s="18"/>
-    </row>
-    <row r="83" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI82" s="17">
+        <v>100</v>
+      </c>
+      <c r="AJ82" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK82" s="7">
+        <v>100</v>
+      </c>
+      <c r="AL82" s="8">
+        <v>1</v>
+      </c>
+      <c r="AM82" s="7">
+        <v>100</v>
+      </c>
+      <c r="AN82" s="8">
+        <v>1</v>
+      </c>
+      <c r="AO82" s="7">
+        <v>100</v>
+      </c>
+      <c r="AP82" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B83" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C83" s="45" t="s">
+      <c r="C83" s="43" t="s">
         <v>49</v>
       </c>
       <c r="D83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E83" s="46" t="s">
+      <c r="E83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="F83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G83" s="46" t="s">
+      <c r="G83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="H83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I83" s="46" t="s">
+      <c r="I83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="J83" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K83" s="45" t="s">
+      <c r="K83" s="43" t="s">
         <v>49</v>
       </c>
       <c r="L83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M83" s="46" t="s">
+      <c r="M83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="N83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="O83" s="46" t="s">
+      <c r="O83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="P83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q83" s="46" t="s">
+      <c r="Q83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="R83" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="S83" s="45" t="s">
+      <c r="S83" s="43" t="s">
         <v>49</v>
       </c>
       <c r="T83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="U83" s="46" t="s">
+      <c r="U83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="V83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="W83" s="46" t="s">
+      <c r="W83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="X83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Y83" s="46" t="s">
+      <c r="Y83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="Z83" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AA83" s="45" t="s">
+      <c r="AA83" s="43" t="s">
         <v>49</v>
       </c>
       <c r="AB83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AC83" s="46" t="s">
+      <c r="AC83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="AD83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AE83" s="46" t="s">
+      <c r="AE83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="AF83" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AG83" s="46" t="s">
+      <c r="AG83" s="44" t="s">
         <v>49</v>
       </c>
       <c r="AH83" s="35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="AI83" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ83" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK83" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL83" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM83" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN83" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO83" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP83" s="35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="2:42" x14ac:dyDescent="0.3">
       <c r="B84" s="25" t="s">
         <v>25</v>
       </c>
@@ -6512,8 +7526,32 @@
       <c r="AF84" s="31"/>
       <c r="AG84" s="32"/>
       <c r="AH84" s="33"/>
-    </row>
-    <row r="85" spans="2:34" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AI84" s="30">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AJ84" s="31">
+        <v>1</v>
+      </c>
+      <c r="AK84" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AL84" s="31">
+        <v>1</v>
+      </c>
+      <c r="AM84" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AN84" s="31">
+        <v>1</v>
+      </c>
+      <c r="AO84" s="32">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="AP84" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:42" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B85" s="27" t="s">
         <v>26</v>
       </c>
@@ -6565,16 +7603,49 @@
       <c r="AF85" s="20"/>
       <c r="AG85" s="21"/>
       <c r="AH85" s="22"/>
+      <c r="AI85" s="19">
+        <v>100</v>
+      </c>
+      <c r="AJ85" s="20">
+        <v>1</v>
+      </c>
+      <c r="AK85" s="21">
+        <v>100</v>
+      </c>
+      <c r="AL85" s="20">
+        <v>1</v>
+      </c>
+      <c r="AM85" s="21">
+        <v>100</v>
+      </c>
+      <c r="AN85" s="20">
+        <v>1</v>
+      </c>
+      <c r="AO85" s="21">
+        <v>100</v>
+      </c>
+      <c r="AP85" s="22">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="AA2:AH2"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="AA4:AH4"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
+  <mergeCells count="39">
+    <mergeCell ref="AI2:AP2"/>
+    <mergeCell ref="AI3:AP3"/>
+    <mergeCell ref="AI4:AP4"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="B71:B79"/>
     <mergeCell ref="S2:Z2"/>
     <mergeCell ref="S3:Z3"/>
@@ -6591,19 +7662,27 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="AA2:AH2"/>
+    <mergeCell ref="AA3:AH3"/>
+    <mergeCell ref="AA4:AH4"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
   </mergeCells>
   <conditionalFormatting sqref="C9:AH85">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>ISBLANK(C9)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI9:AP83">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>ISBLANK(AI9)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI84:AP85">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>ISBLANK(C9)</formula>
+      <formula>ISBLANK(AI84)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6654,16 +7733,16 @@
       </c>
     </row>
     <row r="3" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="64"/>
       <c r="L3" s="36" t="s">
         <v>35</v>
       </c>
@@ -6684,58 +7763,58 @@
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="56" t="s">
+      <c r="D5" s="73"/>
+      <c r="E5" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="56" t="s">
+      <c r="F5" s="73"/>
+      <c r="G5" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="56" t="s">
+      <c r="H5" s="73"/>
+      <c r="I5" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="57"/>
+      <c r="J5" s="75"/>
       <c r="L5" s="38"/>
     </row>
     <row r="6" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="53"/>
-      <c r="D6" s="54">
+      <c r="C6" s="51"/>
+      <c r="D6" s="52">
         <v>43739</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="54">
+      <c r="E6" s="46"/>
+      <c r="F6" s="52">
         <v>43739</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="54">
+      <c r="G6" s="46"/>
+      <c r="H6" s="52">
         <v>43739</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49">
+      <c r="I6" s="46"/>
+      <c r="J6" s="47">
         <v>43739</v>
       </c>
       <c r="L6" s="38"/>
     </row>
     <row r="7" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="50"/>
-      <c r="D7" s="51">
+      <c r="C7" s="48"/>
+      <c r="D7" s="49">
         <v>43738</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="51">
+      <c r="E7" s="46"/>
+      <c r="F7" s="49">
         <v>43738</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="51">
+      <c r="G7" s="46"/>
+      <c r="H7" s="49">
         <v>43738</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="49">
+      <c r="I7" s="46"/>
+      <c r="J7" s="47">
         <v>43738</v>
       </c>
       <c r="L7" s="38"/>

</xml_diff>

<commit_message>
Update Terrain Modification, Volume Calculator and initiate Connectivity
</commit_message>
<xml_diff>
--- a/.site_packages/templates/Fish.xlsx
+++ b/.site_packages/templates/Fish.xlsx
@@ -431,9 +431,6 @@
     <t>All Aquatic</t>
   </si>
   <si>
-    <t>Whetted area</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -443,13 +440,16 @@
     <t>DO NOT MODIFY LIFESTAGE NAMES</t>
   </si>
   <si>
-    <t>hydrologic year</t>
-  </si>
-  <si>
     <t>depth &gt; x</t>
   </si>
   <si>
     <t>velocity &gt; x</t>
+  </si>
+  <si>
+    <t>Wetted area</t>
+  </si>
+  <si>
+    <t>hydrological year</t>
   </si>
 </sst>
 </file>
@@ -1620,15 +1620,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1656,6 +1647,18 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1668,16 +1671,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2048,7 +2048,7 @@
   <dimension ref="B1:AP85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO6" sqref="AO6"/>
+      <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2067,16 +2067,16 @@
       <c r="B1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="58"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="75"/>
       <c r="K1" s="41" t="s">
         <v>43</v>
       </c>
@@ -2111,7 +2111,7 @@
       <c r="V1" s="54"/>
       <c r="W1" s="54"/>
       <c r="X1" s="54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y1" s="54"/>
       <c r="Z1" s="54"/>
@@ -2136,247 +2136,247 @@
       <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="59" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="59" t="s">
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="59" t="s">
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="61"/>
-      <c r="AI2" s="59" t="s">
+      <c r="AB2" s="57"/>
+      <c r="AC2" s="57"/>
+      <c r="AD2" s="57"/>
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="57"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="60"/>
-      <c r="AP2" s="61"/>
+      <c r="AJ2" s="57"/>
+      <c r="AK2" s="57"/>
+      <c r="AL2" s="57"/>
+      <c r="AM2" s="57"/>
+      <c r="AN2" s="57"/>
+      <c r="AO2" s="57"/>
+      <c r="AP2" s="58"/>
     </row>
     <row r="3" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="62" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="62" t="s">
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="63"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ3" s="63"/>
-      <c r="AK3" s="63"/>
-      <c r="AL3" s="63"/>
-      <c r="AM3" s="63"/>
-      <c r="AN3" s="63"/>
-      <c r="AO3" s="63"/>
-      <c r="AP3" s="64"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
+      <c r="AF3" s="60"/>
+      <c r="AG3" s="60"/>
+      <c r="AH3" s="61"/>
+      <c r="AI3" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ3" s="60"/>
+      <c r="AK3" s="60"/>
+      <c r="AL3" s="60"/>
+      <c r="AM3" s="60"/>
+      <c r="AN3" s="60"/>
+      <c r="AO3" s="60"/>
+      <c r="AP3" s="61"/>
     </row>
     <row r="4" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="66"/>
-      <c r="W4" s="66"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="67"/>
-      <c r="AA4" s="65" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="63"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="67"/>
-      <c r="AI4" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ4" s="66"/>
-      <c r="AK4" s="66"/>
-      <c r="AL4" s="66"/>
-      <c r="AM4" s="66"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="67"/>
+      <c r="AB4" s="63"/>
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="63"/>
+      <c r="AE4" s="63"/>
+      <c r="AF4" s="63"/>
+      <c r="AG4" s="63"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ4" s="63"/>
+      <c r="AK4" s="63"/>
+      <c r="AL4" s="63"/>
+      <c r="AM4" s="63"/>
+      <c r="AN4" s="63"/>
+      <c r="AO4" s="63"/>
+      <c r="AP4" s="64"/>
     </row>
     <row r="5" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74" t="s">
+      <c r="D5" s="66"/>
+      <c r="E5" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="74" t="s">
+      <c r="F5" s="66"/>
+      <c r="G5" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74" t="s">
+      <c r="H5" s="66"/>
+      <c r="I5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="75"/>
-      <c r="K5" s="72" t="s">
+      <c r="J5" s="68"/>
+      <c r="K5" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="73"/>
-      <c r="M5" s="74" t="s">
+      <c r="L5" s="66"/>
+      <c r="M5" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="73"/>
-      <c r="O5" s="74" t="s">
+      <c r="N5" s="66"/>
+      <c r="O5" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="74" t="s">
+      <c r="P5" s="66"/>
+      <c r="Q5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="75"/>
-      <c r="S5" s="72" t="s">
+      <c r="R5" s="68"/>
+      <c r="S5" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="73"/>
-      <c r="U5" s="74" t="s">
+      <c r="T5" s="66"/>
+      <c r="U5" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="73"/>
-      <c r="W5" s="74" t="s">
+      <c r="V5" s="66"/>
+      <c r="W5" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="74" t="s">
+      <c r="X5" s="66"/>
+      <c r="Y5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="Z5" s="75"/>
-      <c r="AA5" s="72" t="s">
+      <c r="Z5" s="68"/>
+      <c r="AA5" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="AB5" s="73"/>
-      <c r="AC5" s="74" t="s">
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AD5" s="73"/>
-      <c r="AE5" s="74" t="s">
+      <c r="AD5" s="66"/>
+      <c r="AE5" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="AF5" s="73"/>
-      <c r="AG5" s="74" t="s">
+      <c r="AF5" s="66"/>
+      <c r="AG5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="72" t="s">
+      <c r="AH5" s="68"/>
+      <c r="AI5" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ5" s="66"/>
+      <c r="AK5" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL5" s="66"/>
+      <c r="AM5" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN5" s="66"/>
+      <c r="AO5" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="AJ5" s="73"/>
-      <c r="AK5" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL5" s="73"/>
-      <c r="AM5" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN5" s="73"/>
-      <c r="AO5" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP5" s="75"/>
+      <c r="AP5" s="68"/>
     </row>
     <row r="6" spans="2:42" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="45" t="s">
@@ -2477,7 +2477,7 @@
       </c>
       <c r="G7" s="46"/>
       <c r="H7" s="49">
-        <v>43769</v>
+        <v>43798</v>
       </c>
       <c r="I7" s="46"/>
       <c r="J7" s="47">
@@ -2549,7 +2549,7 @@
       </c>
     </row>
     <row r="8" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="69" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="43" t="s">
@@ -2674,7 +2674,7 @@
       </c>
     </row>
     <row r="9" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B9" s="69"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="30">
         <v>0.22</v>
       </c>
@@ -2773,7 +2773,7 @@
       </c>
     </row>
     <row r="10" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B10" s="69"/>
+      <c r="B10" s="70"/>
       <c r="C10" s="15">
         <v>0.85</v>
       </c>
@@ -2872,7 +2872,7 @@
       </c>
     </row>
     <row r="11" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B11" s="69"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="15">
         <v>1.3</v>
       </c>
@@ -2959,7 +2959,7 @@
       </c>
     </row>
     <row r="12" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B12" s="69"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="15">
         <v>1.55</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
     </row>
     <row r="13" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B13" s="69"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="15">
         <v>2.95</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="AP13" s="16"/>
     </row>
     <row r="14" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B14" s="69"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="15">
         <v>3.25</v>
       </c>
@@ -3196,7 +3196,7 @@
       <c r="AP14" s="16"/>
     </row>
     <row r="15" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B15" s="69"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="15">
         <v>5.32</v>
       </c>
@@ -3271,7 +3271,7 @@
       <c r="AP15" s="16"/>
     </row>
     <row r="16" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B16" s="69"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="15"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5">
@@ -3338,7 +3338,7 @@
       <c r="AP16" s="16"/>
     </row>
     <row r="17" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B17" s="69"/>
+      <c r="B17" s="70"/>
       <c r="C17" s="15"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5">
@@ -3401,7 +3401,7 @@
       <c r="AP17" s="16"/>
     </row>
     <row r="18" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B18" s="69"/>
+      <c r="B18" s="70"/>
       <c r="C18" s="15"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5">
@@ -3464,7 +3464,7 @@
       <c r="AP18" s="16"/>
     </row>
     <row r="19" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B19" s="69"/>
+      <c r="B19" s="70"/>
       <c r="C19" s="15"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5">
@@ -3523,7 +3523,7 @@
       <c r="AP19" s="16"/>
     </row>
     <row r="20" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B20" s="69"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="15"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5">
@@ -3582,7 +3582,7 @@
       <c r="AP20" s="16"/>
     </row>
     <row r="21" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B21" s="69"/>
+      <c r="B21" s="70"/>
       <c r="C21" s="15"/>
       <c r="D21" s="6"/>
       <c r="E21" s="5">
@@ -3641,7 +3641,7 @@
       <c r="AP21" s="16"/>
     </row>
     <row r="22" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B22" s="69"/>
+      <c r="B22" s="70"/>
       <c r="C22" s="15"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5">
@@ -3700,7 +3700,7 @@
       <c r="AP22" s="16"/>
     </row>
     <row r="23" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B23" s="69"/>
+      <c r="B23" s="70"/>
       <c r="C23" s="15"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5">
@@ -3759,7 +3759,7 @@
       <c r="AP23" s="16"/>
     </row>
     <row r="24" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B24" s="69"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="15"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
@@ -3814,7 +3814,7 @@
       <c r="AP24" s="16"/>
     </row>
     <row r="25" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B25" s="69"/>
+      <c r="B25" s="70"/>
       <c r="C25" s="15"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
@@ -3869,7 +3869,7 @@
       <c r="AP25" s="16"/>
     </row>
     <row r="26" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B26" s="69"/>
+      <c r="B26" s="70"/>
       <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
@@ -3920,7 +3920,7 @@
       <c r="AP26" s="16"/>
     </row>
     <row r="27" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B27" s="69"/>
+      <c r="B27" s="70"/>
       <c r="C27" s="15"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
@@ -3971,7 +3971,7 @@
       <c r="AP27" s="16"/>
     </row>
     <row r="28" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B28" s="69"/>
+      <c r="B28" s="70"/>
       <c r="C28" s="15"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
@@ -4022,7 +4022,7 @@
       <c r="AP28" s="16"/>
     </row>
     <row r="29" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B29" s="69"/>
+      <c r="B29" s="70"/>
       <c r="C29" s="15"/>
       <c r="D29" s="6"/>
       <c r="E29" s="5"/>
@@ -4073,7 +4073,7 @@
       <c r="AP29" s="16"/>
     </row>
     <row r="30" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B30" s="69"/>
+      <c r="B30" s="70"/>
       <c r="C30" s="15"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
@@ -4124,7 +4124,7 @@
       <c r="AP30" s="16"/>
     </row>
     <row r="31" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B31" s="69"/>
+      <c r="B31" s="70"/>
       <c r="C31" s="15"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
@@ -4175,7 +4175,7 @@
       <c r="AP31" s="16"/>
     </row>
     <row r="32" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B32" s="69"/>
+      <c r="B32" s="70"/>
       <c r="C32" s="15"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
@@ -4226,7 +4226,7 @@
       <c r="AP32" s="16"/>
     </row>
     <row r="33" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B33" s="69"/>
+      <c r="B33" s="70"/>
       <c r="C33" s="15"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
@@ -4277,7 +4277,7 @@
       <c r="AP33" s="16"/>
     </row>
     <row r="34" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B34" s="69"/>
+      <c r="B34" s="70"/>
       <c r="C34" s="15"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
@@ -4328,7 +4328,7 @@
       <c r="AP34" s="16"/>
     </row>
     <row r="35" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B35" s="69"/>
+      <c r="B35" s="70"/>
       <c r="C35" s="15"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
@@ -4379,7 +4379,7 @@
       <c r="AP35" s="16"/>
     </row>
     <row r="36" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B36" s="71"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="17"/>
       <c r="D36" s="8"/>
       <c r="E36" s="7"/>
@@ -4430,7 +4430,7 @@
       <c r="AP36" s="18"/>
     </row>
     <row r="37" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="69" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="43" t="s">
@@ -4555,7 +4555,7 @@
       </c>
     </row>
     <row r="38" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B38" s="69"/>
+      <c r="B38" s="70"/>
       <c r="C38" s="30">
         <v>0.25</v>
       </c>
@@ -4654,7 +4654,7 @@
       </c>
     </row>
     <row r="39" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B39" s="69"/>
+      <c r="B39" s="70"/>
       <c r="C39" s="15">
         <v>0.45</v>
       </c>
@@ -4753,7 +4753,7 @@
       </c>
     </row>
     <row r="40" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B40" s="69"/>
+      <c r="B40" s="70"/>
       <c r="C40" s="15">
         <v>0.65</v>
       </c>
@@ -4840,7 +4840,7 @@
       <c r="AP40" s="16"/>
     </row>
     <row r="41" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B41" s="69"/>
+      <c r="B41" s="70"/>
       <c r="C41" s="15">
         <v>0.75</v>
       </c>
@@ -4919,7 +4919,7 @@
       <c r="AP41" s="16"/>
     </row>
     <row r="42" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B42" s="69"/>
+      <c r="B42" s="70"/>
       <c r="C42" s="15">
         <v>0.95</v>
       </c>
@@ -4994,7 +4994,7 @@
       <c r="AP42" s="16"/>
     </row>
     <row r="43" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B43" s="69"/>
+      <c r="B43" s="70"/>
       <c r="C43" s="15">
         <v>2</v>
       </c>
@@ -5065,7 +5065,7 @@
       <c r="AP43" s="16"/>
     </row>
     <row r="44" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B44" s="69"/>
+      <c r="B44" s="70"/>
       <c r="C44" s="15">
         <v>3</v>
       </c>
@@ -5128,7 +5128,7 @@
       <c r="AP44" s="16"/>
     </row>
     <row r="45" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B45" s="69"/>
+      <c r="B45" s="70"/>
       <c r="C45" s="15">
         <v>4.8</v>
       </c>
@@ -5191,7 +5191,7 @@
       <c r="AP45" s="16"/>
     </row>
     <row r="46" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B46" s="69"/>
+      <c r="B46" s="70"/>
       <c r="C46" s="15">
         <v>7.8</v>
       </c>
@@ -5250,7 +5250,7 @@
       <c r="AP46" s="16"/>
     </row>
     <row r="47" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B47" s="69"/>
+      <c r="B47" s="70"/>
       <c r="C47" s="15">
         <v>7.9</v>
       </c>
@@ -5309,7 +5309,7 @@
       <c r="AP47" s="16"/>
     </row>
     <row r="48" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B48" s="69"/>
+      <c r="B48" s="70"/>
       <c r="C48" s="15"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5">
@@ -5360,7 +5360,7 @@
       <c r="AP48" s="16"/>
     </row>
     <row r="49" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B49" s="69"/>
+      <c r="B49" s="70"/>
       <c r="C49" s="15"/>
       <c r="D49" s="6"/>
       <c r="E49" s="5">
@@ -5411,7 +5411,7 @@
       <c r="AP49" s="16"/>
     </row>
     <row r="50" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B50" s="69"/>
+      <c r="B50" s="70"/>
       <c r="C50" s="15"/>
       <c r="D50" s="6"/>
       <c r="E50" s="5">
@@ -5462,7 +5462,7 @@
       <c r="AP50" s="16"/>
     </row>
     <row r="51" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B51" s="69"/>
+      <c r="B51" s="70"/>
       <c r="C51" s="15"/>
       <c r="D51" s="6"/>
       <c r="E51" s="5">
@@ -5513,7 +5513,7 @@
       <c r="AP51" s="16"/>
     </row>
     <row r="52" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B52" s="69"/>
+      <c r="B52" s="70"/>
       <c r="C52" s="15"/>
       <c r="D52" s="6"/>
       <c r="E52" s="5">
@@ -5564,7 +5564,7 @@
       <c r="AP52" s="16"/>
     </row>
     <row r="53" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B53" s="69"/>
+      <c r="B53" s="70"/>
       <c r="C53" s="15"/>
       <c r="D53" s="6"/>
       <c r="E53" s="5">
@@ -5615,7 +5615,7 @@
       <c r="AP53" s="16"/>
     </row>
     <row r="54" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B54" s="69"/>
+      <c r="B54" s="70"/>
       <c r="C54" s="15"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5">
@@ -5662,7 +5662,7 @@
       <c r="AP54" s="16"/>
     </row>
     <row r="55" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B55" s="69"/>
+      <c r="B55" s="70"/>
       <c r="C55" s="15"/>
       <c r="D55" s="6"/>
       <c r="E55" s="5">
@@ -5709,7 +5709,7 @@
       <c r="AP55" s="16"/>
     </row>
     <row r="56" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B56" s="69"/>
+      <c r="B56" s="70"/>
       <c r="C56" s="15"/>
       <c r="D56" s="6"/>
       <c r="E56" s="5">
@@ -5756,7 +5756,7 @@
       <c r="AP56" s="16"/>
     </row>
     <row r="57" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B57" s="69"/>
+      <c r="B57" s="70"/>
       <c r="C57" s="15"/>
       <c r="D57" s="6"/>
       <c r="E57" s="5">
@@ -5803,7 +5803,7 @@
       <c r="AP57" s="16"/>
     </row>
     <row r="58" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B58" s="69"/>
+      <c r="B58" s="70"/>
       <c r="C58" s="15"/>
       <c r="D58" s="6"/>
       <c r="E58" s="5">
@@ -5850,7 +5850,7 @@
       <c r="AP58" s="16"/>
     </row>
     <row r="59" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B59" s="69"/>
+      <c r="B59" s="70"/>
       <c r="C59" s="15"/>
       <c r="D59" s="6"/>
       <c r="E59" s="5">
@@ -5897,7 +5897,7 @@
       <c r="AP59" s="16"/>
     </row>
     <row r="60" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B60" s="69"/>
+      <c r="B60" s="70"/>
       <c r="C60" s="15"/>
       <c r="D60" s="6"/>
       <c r="E60" s="5">
@@ -5944,7 +5944,7 @@
       <c r="AP60" s="16"/>
     </row>
     <row r="61" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B61" s="69"/>
+      <c r="B61" s="70"/>
       <c r="C61" s="15"/>
       <c r="D61" s="6"/>
       <c r="E61" s="5">
@@ -5991,7 +5991,7 @@
       <c r="AP61" s="16"/>
     </row>
     <row r="62" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B62" s="69"/>
+      <c r="B62" s="70"/>
       <c r="C62" s="15"/>
       <c r="D62" s="6"/>
       <c r="E62" s="5">
@@ -6038,7 +6038,7 @@
       <c r="AP62" s="16"/>
     </row>
     <row r="63" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B63" s="69"/>
+      <c r="B63" s="70"/>
       <c r="C63" s="15"/>
       <c r="D63" s="6"/>
       <c r="E63" s="5">
@@ -6085,7 +6085,7 @@
       <c r="AP63" s="16"/>
     </row>
     <row r="64" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B64" s="69"/>
+      <c r="B64" s="70"/>
       <c r="C64" s="15"/>
       <c r="D64" s="6"/>
       <c r="E64" s="5">
@@ -6132,7 +6132,7 @@
       <c r="AP64" s="16"/>
     </row>
     <row r="65" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B65" s="69"/>
+      <c r="B65" s="70"/>
       <c r="C65" s="15"/>
       <c r="D65" s="6"/>
       <c r="E65" s="5">
@@ -6179,7 +6179,7 @@
       <c r="AP65" s="16"/>
     </row>
     <row r="66" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B66" s="69"/>
+      <c r="B66" s="70"/>
       <c r="C66" s="15"/>
       <c r="D66" s="6"/>
       <c r="E66" s="5">
@@ -6226,7 +6226,7 @@
       <c r="AP66" s="16"/>
     </row>
     <row r="67" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B67" s="69"/>
+      <c r="B67" s="70"/>
       <c r="C67" s="15"/>
       <c r="D67" s="6"/>
       <c r="E67" s="5">
@@ -6273,7 +6273,7 @@
       <c r="AP67" s="16"/>
     </row>
     <row r="68" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B68" s="69"/>
+      <c r="B68" s="70"/>
       <c r="C68" s="15"/>
       <c r="D68" s="6"/>
       <c r="E68" s="5">
@@ -6320,7 +6320,7 @@
       <c r="AP68" s="16"/>
     </row>
     <row r="69" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B69" s="69"/>
+      <c r="B69" s="70"/>
       <c r="C69" s="15"/>
       <c r="D69" s="6"/>
       <c r="E69" s="5">
@@ -6367,7 +6367,7 @@
       <c r="AP69" s="16"/>
     </row>
     <row r="70" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B70" s="71"/>
+      <c r="B70" s="72"/>
       <c r="C70" s="17"/>
       <c r="D70" s="8"/>
       <c r="E70" s="7">
@@ -6414,7 +6414,7 @@
       <c r="AP70" s="18"/>
     </row>
     <row r="71" spans="2:42" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="68" t="s">
+      <c r="B71" s="69" t="s">
         <v>17</v>
       </c>
       <c r="C71" s="43" t="s">
@@ -6539,7 +6539,7 @@
       </c>
     </row>
     <row r="72" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B72" s="69"/>
+      <c r="B72" s="70"/>
       <c r="C72" s="30">
         <v>0.10170583333333333</v>
       </c>
@@ -6626,7 +6626,7 @@
       </c>
     </row>
     <row r="73" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B73" s="69"/>
+      <c r="B73" s="70"/>
       <c r="C73" s="15">
         <v>0.10498666666666666</v>
       </c>
@@ -6713,7 +6713,7 @@
       </c>
     </row>
     <row r="74" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B74" s="69"/>
+      <c r="B74" s="70"/>
       <c r="C74" s="15">
         <v>0.63976250000000001</v>
       </c>
@@ -6784,7 +6784,7 @@
       <c r="AP74" s="16"/>
     </row>
     <row r="75" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B75" s="69"/>
+      <c r="B75" s="70"/>
       <c r="C75" s="15">
         <v>0.6430433333333333</v>
       </c>
@@ -6855,7 +6855,7 @@
       <c r="AP75" s="16"/>
     </row>
     <row r="76" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B76" s="69"/>
+      <c r="B76" s="70"/>
       <c r="C76" s="15"/>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
@@ -6914,7 +6914,7 @@
       <c r="AP76" s="16"/>
     </row>
     <row r="77" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B77" s="70"/>
+      <c r="B77" s="71"/>
       <c r="C77" s="28"/>
       <c r="D77" s="10"/>
       <c r="E77" s="9"/>
@@ -6969,7 +6969,7 @@
       <c r="AP77" s="29"/>
     </row>
     <row r="78" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B78" s="70"/>
+      <c r="B78" s="71"/>
       <c r="C78" s="28"/>
       <c r="D78" s="10"/>
       <c r="E78" s="9"/>
@@ -7020,7 +7020,7 @@
       <c r="AP78" s="29"/>
     </row>
     <row r="79" spans="2:42" x14ac:dyDescent="0.3">
-      <c r="B79" s="71"/>
+      <c r="B79" s="72"/>
       <c r="C79" s="17"/>
       <c r="D79" s="8"/>
       <c r="E79" s="7"/>
@@ -7630,22 +7630,13 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="AI2:AP2"/>
-    <mergeCell ref="AI3:AP3"/>
-    <mergeCell ref="AI4:AP4"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="AA2:AH2"/>
+    <mergeCell ref="AA3:AH3"/>
+    <mergeCell ref="AA4:AH4"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C4:J4"/>
     <mergeCell ref="B71:B79"/>
     <mergeCell ref="S2:Z2"/>
     <mergeCell ref="S3:Z3"/>
@@ -7662,13 +7653,22 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="O5:P5"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="AA2:AH2"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="AA4:AH4"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AI2:AP2"/>
+    <mergeCell ref="AI3:AP3"/>
+    <mergeCell ref="AI4:AP4"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AP5"/>
   </mergeCells>
   <conditionalFormatting sqref="C9:AH85">
     <cfRule type="expression" dxfId="5" priority="3">
@@ -7733,16 +7733,16 @@
       </c>
     </row>
     <row r="3" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
       <c r="L3" s="36" t="s">
         <v>35</v>
       </c>
@@ -7763,22 +7763,22 @@
       </c>
     </row>
     <row r="5" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74" t="s">
+      <c r="D5" s="66"/>
+      <c r="E5" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="74" t="s">
+      <c r="F5" s="66"/>
+      <c r="G5" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74" t="s">
+      <c r="H5" s="66"/>
+      <c r="I5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="75"/>
+      <c r="J5" s="68"/>
       <c r="L5" s="38"/>
     </row>
     <row r="6" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">

</xml_diff>